<commit_message>
add shareprice and earnings progress
</commit_message>
<xml_diff>
--- a/networth_progress_example.xlsx
+++ b/networth_progress_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\OneDrive\Documents\dev\strategy1835\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D09A90D-0353-4DA3-8819-FE816E7BAE9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755154A7-82B7-46AF-9DBC-73EB39CFD8F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{4194B167-A74A-476C-A945-F3B3FB62131B}"/>
   </bookViews>
@@ -32,18 +32,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>Dan</t>
-  </si>
-  <si>
-    <t>Hakko</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>Pep</t>
-  </si>
   <si>
     <t>OR1.1</t>
   </si>
@@ -91,6 +79,18 @@
   </si>
   <si>
     <t>OR9.1</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P4</t>
   </si>
 </sst>
 </file>
@@ -160,6 +160,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Net worth</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -204,7 +229,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Dan</c:v>
+                  <c:v>P1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -414,7 +439,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hakko</c:v>
+                  <c:v>P2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -624,7 +649,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Peter</c:v>
+                  <c:v>P3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -834,7 +859,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Pep</c:v>
+                  <c:v>P4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2122,23 +2147,23 @@
   <dimension ref="A2:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2146,7 +2171,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>475</v>
@@ -2166,7 +2191,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>389</v>
@@ -2186,7 +2211,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>444</v>
@@ -2206,7 +2231,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>558</v>
@@ -2226,7 +2251,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>720</v>
@@ -2246,7 +2271,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>936</v>
@@ -2266,7 +2291,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>1263</v>
@@ -2286,7 +2311,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>1580</v>
@@ -2306,7 +2331,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>1988</v>
@@ -2326,7 +2351,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>2596</v>
@@ -2346,7 +2371,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>3023</v>
@@ -2366,7 +2391,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>3625</v>
@@ -2386,7 +2411,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>4082</v>
@@ -2406,7 +2431,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>4784</v>
@@ -2426,7 +2451,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>5484</v>
@@ -2446,7 +2471,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>6615</v>

</xml_diff>